<commit_message>
modified to work on any number of elements
</commit_message>
<xml_diff>
--- a/Documentation/ExecutionTimes.xlsx
+++ b/Documentation/ExecutionTimes.xlsx
@@ -5,27 +5,37 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Facultate\3.2\Algoritmi paraleli si distribuiti\RadixSort\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Facultate\3.2\Algoritmi paraleli si distribuiti\RadixSortProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E2A3C3-F51F-4213-94A0-2A7999763567}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1B17D3-92BA-46B2-8D11-AE3EEF5DBCE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7C64941E-466C-4937-94FB-CC73CF9B5C7A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7C64941E-466C-4937-94FB-CC73CF9B5C7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>Std sort</t>
   </si>
@@ -49,6 +59,30 @@
   </si>
   <si>
     <t>No.elements  (lg)</t>
+  </si>
+  <si>
+    <t>PRadB</t>
+  </si>
+  <si>
+    <t>PRadC Partial</t>
+  </si>
+  <si>
+    <t>PRadC Full</t>
+  </si>
+  <si>
+    <t>buffer full</t>
+  </si>
+  <si>
+    <t>No.processes</t>
+  </si>
+  <si>
+    <t>not dividable</t>
+  </si>
+  <si>
+    <t>no dividable</t>
+  </si>
+  <si>
+    <t>error</t>
   </si>
 </sst>
 </file>
@@ -1519,6 +1553,1382 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Times for 8</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> processes</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Radix sort(ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.1299999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.63E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.6500000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54659999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.3979999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>54.410699999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>533.55799999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5416.76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D130-4882-B68B-2762F1E015DA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PRadC Partial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.2965</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2383000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2073999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.1196000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.3035</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>155.203</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>837.77599999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4242</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D130-4882-B68B-2762F1E015DA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PRadC Full</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.3223</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4945999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2712000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7629999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.8807999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>317.24799999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3786.28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D130-4882-B68B-2762F1E015DA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1250538223"/>
+        <c:axId val="1250558191"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1250538223"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of elements to sort</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1250558191"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1250558191"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>milliseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1250538223"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Times</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> for 10^5 elements</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PRadC Partial</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$G$2:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$H$2:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.3421000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5895999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.1337000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20.511399999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27.102599999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.796099999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.704699999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>677.76300000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-86C9-4258-B74F-969833D9B2D2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PRadC Full</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$G$2:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$I$2:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.2370000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8740000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.8064999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.4264999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.3761000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>82.308300000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>491.66500000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1679.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-86C9-4258-B74F-969833D9B2D2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1250516175"/>
+        <c:axId val="1250516591"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1250516175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>number of threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1250516591"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1250516591"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>milliseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1250516175"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1599,6 +3009,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2116,6 +3606,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2688,6 +5210,83 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E23D64D-8EF1-46A4-825C-111A1EF83188}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92CB4654-5BC6-4E90-9787-9680DD9A94D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70C17738-A497-4412-B6D6-8CEC2647745E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3007,8 +5606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F509CFBE-C125-4605-8B68-5D60578F46EE}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:I9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3285,4 +5884,288 @@
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD8A123-4E93-4394-9044-D7BF87729DC0}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>2.1299999999999999E-2</v>
+      </c>
+      <c r="C2">
+        <v>2.2965</v>
+      </c>
+      <c r="D2">
+        <v>1.3223</v>
+      </c>
+      <c r="E2">
+        <v>2.0331999999999999</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>5.3421000000000003</v>
+      </c>
+      <c r="I2">
+        <v>4.2370000000000001</v>
+      </c>
+      <c r="J2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>2.63E-2</v>
+      </c>
+      <c r="C3">
+        <v>2.2383000000000002</v>
+      </c>
+      <c r="D3">
+        <v>1.4945999999999999</v>
+      </c>
+      <c r="E3">
+        <v>3.863</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>5.5895999999999999</v>
+      </c>
+      <c r="I3">
+        <v>3.8740000000000001</v>
+      </c>
+      <c r="J3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1000</v>
+      </c>
+      <c r="B4">
+        <v>6.6500000000000004E-2</v>
+      </c>
+      <c r="C4">
+        <v>2.2073999999999998</v>
+      </c>
+      <c r="D4">
+        <v>1.2712000000000001</v>
+      </c>
+      <c r="E4">
+        <v>4.0730000000000004</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>6.1337000000000002</v>
+      </c>
+      <c r="I4">
+        <v>5.8064999999999998</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>10000</v>
+      </c>
+      <c r="B5">
+        <v>0.54659999999999997</v>
+      </c>
+      <c r="C5">
+        <v>6.1196000000000002</v>
+      </c>
+      <c r="D5">
+        <v>1.7629999999999999</v>
+      </c>
+      <c r="E5">
+        <v>5.8156999999999996</v>
+      </c>
+      <c r="G5">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>20.511399999999998</v>
+      </c>
+      <c r="I5">
+        <v>5.4264999999999999</v>
+      </c>
+      <c r="J5">
+        <v>9.2134999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>100000</v>
+      </c>
+      <c r="B6">
+        <v>5.3979999999999997</v>
+      </c>
+      <c r="C6">
+        <v>27.3035</v>
+      </c>
+      <c r="D6">
+        <v>4.8807999999999998</v>
+      </c>
+      <c r="E6">
+        <v>9.3579000000000008</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>27.102599999999999</v>
+      </c>
+      <c r="I6">
+        <v>6.3761000000000001</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1000000</v>
+      </c>
+      <c r="B7">
+        <v>54.410699999999999</v>
+      </c>
+      <c r="C7">
+        <v>155.203</v>
+      </c>
+      <c r="D7">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7">
+        <v>16</v>
+      </c>
+      <c r="H7">
+        <v>14.796099999999999</v>
+      </c>
+      <c r="I7">
+        <v>82.308300000000003</v>
+      </c>
+      <c r="J7">
+        <v>153.11600000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>10000000</v>
+      </c>
+      <c r="B8">
+        <v>533.55799999999999</v>
+      </c>
+      <c r="C8">
+        <v>837.77599999999995</v>
+      </c>
+      <c r="D8">
+        <v>317.24799999999999</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8">
+        <v>32</v>
+      </c>
+      <c r="H8">
+        <v>23.704699999999999</v>
+      </c>
+      <c r="I8">
+        <v>491.66500000000002</v>
+      </c>
+      <c r="J8">
+        <v>1860.98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>100000000</v>
+      </c>
+      <c r="B9">
+        <v>5416.76</v>
+      </c>
+      <c r="C9">
+        <v>4242</v>
+      </c>
+      <c r="D9">
+        <v>3786.28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9">
+        <v>64</v>
+      </c>
+      <c r="H9">
+        <v>677.76300000000003</v>
+      </c>
+      <c r="I9">
+        <v>1679.5</v>
+      </c>
+      <c r="J9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>